<commit_message>
filtros y reportes de compras
</commit_message>
<xml_diff>
--- a/export_pagos.xlsx
+++ b/export_pagos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Num. Pago</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>Efectivo</t>
+  </si>
+  <si>
+    <t>$300.00</t>
+  </si>
+  <si>
+    <t>2023-07-07</t>
+  </si>
+  <si>
+    <t>Transferencia</t>
+  </si>
+  <si>
+    <t>Banco Bolivariano</t>
   </si>
 </sst>
 </file>
@@ -405,7 +417,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +500,39 @@
       <c r="J2"/>
       <c r="K2"/>
     </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3"/>
+      <c r="I3">
+        <v>23123</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
filtros y reportes cobros, mejoras en cobros y pagos
</commit_message>
<xml_diff>
--- a/export_pagos.xlsx
+++ b/export_pagos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Num. Pago</t>
   </si>
@@ -48,36 +48,6 @@
   </si>
   <si>
     <t>Fecha Mov.</t>
-  </si>
-  <si>
-    <t>John Marcos Davis Cedeño</t>
-  </si>
-  <si>
-    <t>111-111-111111111</t>
-  </si>
-  <si>
-    <t>$672.00</t>
-  </si>
-  <si>
-    <t>$372.00</t>
-  </si>
-  <si>
-    <t>2023-06-17</t>
-  </si>
-  <si>
-    <t>Efectivo</t>
-  </si>
-  <si>
-    <t>$300.00</t>
-  </si>
-  <si>
-    <t>2023-07-07</t>
-  </si>
-  <si>
-    <t>Transferencia</t>
-  </si>
-  <si>
-    <t>Banco Bolivariano</t>
   </si>
 </sst>
 </file>
@@ -417,7 +387,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,66 +443,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3"/>
-      <c r="I3">
-        <v>23123</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>